<commit_message>
Politicas e template para registro de nao conformidades
</commit_message>
<xml_diff>
--- a/Etapa 1/Processo de qualidade.xlsx
+++ b/Etapa 1/Processo de qualidade.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UFG\QUALIDADE DE SOFTWARE\QualidadeSoftware\Etapa 1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC13294-FC46-4E29-837A-8DC00DCC5C71}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Papeis</t>
   </si>
@@ -161,11 +167,20 @@
   <si>
     <t>Relatório</t>
   </si>
+  <si>
+    <t>Comunicar resultado da avaliação de qualidade</t>
+  </si>
+  <si>
+    <t>Registrar não conformidades</t>
+  </si>
+  <si>
+    <t>Comunicar resultados da avaliação da qualidade</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -211,6 +226,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -218,7 +236,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -256,9 +274,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,9 +309,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,9 +361,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -501,23 +553,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,20 +577,20 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -546,51 +598,56 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>43</v>
       </c>
     </row>
@@ -600,21 +657,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D26" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="128.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="170.28515625" customWidth="1"/>
+    <col min="4" max="4" width="128.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -625,7 +682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -642,17 +699,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -663,112 +720,123 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>19</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>20</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>24</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D21" t="s">
         <v>25</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E21" t="s">
         <v>26</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F21" t="s">
         <v>27</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="3:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
+    <row r="22" spans="1:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>